<commit_message>
added photo count to sheets
</commit_message>
<xml_diff>
--- a/coverage.xlsx
+++ b/coverage.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">coverage (m)</t>
   </si>
@@ -71,6 +72,12 @@
   </si>
   <si>
     <t xml:space="preserve">residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHOTOS</t>
   </si>
 </sst>
 </file>
@@ -81,7 +88,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -101,6 +108,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,12 +158,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -173,7 +190,7 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -442,4 +459,132 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>2011</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2014</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>8318</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>2015</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>27009</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2016</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>33789</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>3938</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>96022</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>512519</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>8539</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1741455</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>